<commit_message>
Lagt til .DS_Store i .gitignore og fjerna unødvendig
</commit_message>
<xml_diff>
--- a/prosjektfiler/LoadFlow_results.xlsx
+++ b/prosjektfiler/LoadFlow_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arntzen/Desktop/IELET2118---Prosjekt-Lastflytanalyse/prosjektfiler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Desktop\IELET2118---Prosjekt-Lastflytanalyse\prosjektfiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FFE118-DCC1-E844-AA12-5BE04146283E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5936FB29-3959-4AD6-AA9B-F00E31047D59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus_information" sheetId="1" r:id="rId1"/>
@@ -87,8 +87,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -112,12 +120,154 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,243 +573,266 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="7">
         <v>1.02</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
         <v>0.78498674092298659</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="7">
         <v>0.27047245420165211</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="8">
         <v>1.0329999999999999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>0.82247761238476069</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>0.30000000000002341</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="8">
         <v>0.13728476230023651</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="8">
         <v>1.0289999999999999</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>0.1035613926270709</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>0.33000000000000962</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="8">
         <v>0.13839357922779169</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <v>0.98499999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
         <v>-5.9080393936706761</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
         <v>0.17999999999942151</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="8">
         <v>0.16744894175991121</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="8">
         <v>0.9693903875069888</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>-7.5832064927970952</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="8">
+        <v>0</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0</v>
+      </c>
+      <c r="F7" s="8">
         <v>0.1000000000513421</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="8">
         <v>5.9999999986285253E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>0.91254234954751878</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>-16.470569404687289</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
         <v>1.049999999915838</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="8">
         <v>0.22499999992401781</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <v>0.91384955883213392</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>-16.169372392524579</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0</v>
+      </c>
+      <c r="F9" s="8">
         <v>0.17999999993589</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="8">
         <v>4.499999999319737E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="8">
         <v>0.92981492874428351</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="8">
         <v>-12.99295728703369</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="F10" s="8">
         <v>0.22500000004211171</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="8">
         <v>4.499999996911086E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
         <v>1.594986740922441</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="8">
         <v>0.71359973748959149</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="8">
         <v>1.554999999945182</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="8">
         <v>0.37499999987261118</v>
       </c>
     </row>
@@ -672,295 +845,321 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="2"/>
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="7">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="7">
         <v>-0.1481371226060835</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <v>-0.1093521991185932</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="7">
         <v>0.14846259060451961</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="7">
         <v>0.1069151366591939</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="7">
         <v>3.2546799843616298E-4</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="7">
         <v>3.4987809831887461E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="8">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>0.15153740939548091</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>3.0369625641026611E-2</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="8">
         <v>-0.1513491560528924</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="8">
         <v>-3.3261637051876063E-2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="8">
         <v>1.8825334258845691E-4</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="8">
         <v>2.023723432825926E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="8">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>0.48134915605289252</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>0.1716552162811244</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="8">
         <v>-0.47606556983556142</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="8">
         <v>-0.12678571033762029</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="8">
         <v>5.2835862173311043E-3</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="8">
         <v>5.6798551836309108E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="8">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
         <v>0.65606556983556219</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
         <v>0.29423465220832962</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="8">
         <v>-0.65391175712690297</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="8">
         <v>-0.27423458363533398</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="8">
         <v>2.15381270865922E-3</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="8">
         <v>2.3691939795251749E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="8">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>0.55391175712690222</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>0.21423458363532871</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="8">
         <v>-0.54789327706383129</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="8">
         <v>-0.13827752503970539</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="8">
         <v>6.0184800630709301E-3</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="8">
         <v>9.6295681009135353E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="8">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>-2.2956621005215019E-2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>-1.1973721173526859E-2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="8">
         <v>2.296458861318177E-2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="8">
         <v>-2.521387437091141E-3</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="8">
         <v>7.9676079667578836E-6</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="8">
         <v>1.2748172746810191E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="8">
         <v>8</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>-0.20296458861318209</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>-4.2478612562908392E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="8">
         <v>0.20408438900926421</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="8">
         <v>4.4189448700229339E-2</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="8">
         <v>1.119800396082143E-3</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="8">
         <v>1.203785425788294E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
         <v>1</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="8">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="8">
         <v>0.43942849810442142</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <v>0.17560000943158011</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="8">
         <v>-0.42908438900926421</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="8">
         <v>-8.9189448700229421E-2</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="8">
         <v>1.0344109095157259E-2</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="8">
         <v>0.1111991727729407</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
         <v>1</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="8">
         <v>6</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="8">
         <v>0.49369536548657278</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
         <v>0.20422464399984999</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="8">
         <v>-0.47915010193095359</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="8">
         <v>-7.4748753786769526E-2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="8">
         <v>1.454526355561914E-2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="8">
         <v>0.15636158322290611</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F13" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="8">
         <v>3.9986740984911173E-2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="8">
         <v>0.46203476903790858</v>
       </c>
     </row>
@@ -973,13 +1172,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1.1907776635489029</v>
       </c>
@@ -1005,7 +1204,7 @@
         <v>-0.18244753366410449</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-0.84292353981057178</v>
       </c>
@@ -1031,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1057,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1083,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1109,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-0.1654065900742264</v>
       </c>
@@ -1135,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1161,7 +1360,7 @@
         <v>-0.39074795671380941</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-0.18244753366410449</v>
       </c>
@@ -1198,9 +1397,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-12.770677314474741</v>
       </c>
@@ -1226,7 +1425,7 @@
         <v>1.961310986889121</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9.0614280529637057</v>
       </c>
@@ -1252,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1278,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1304,7 +1503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1330,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.7781208432979341</v>
       </c>
@@ -1356,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1382,7 +1581,7 @@
         <v>4.2005405346734577</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.961310986889121</v>
       </c>

</xml_diff>

<commit_message>
Oppdatart System_data for 4b)
</commit_message>
<xml_diff>
--- a/prosjektfiler/LoadFlow_results.xlsx
+++ b/prosjektfiler/LoadFlow_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arntzen/Desktop/IELET2118---Prosjekt-Lastflytanalyse/prosjektfiler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Desktop\IELET2118---Prosjekt-Lastflytanalyse\prosjektfiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46357E13-CF6B-514E-B364-EEE3D8AE1530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF84362-B720-49EC-AE4C-C607C1FC2CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus_information" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
     <sheet name="Ybus_real_part" sheetId="3" r:id="rId3"/>
     <sheet name="Ybus_imaginary_part" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -74,8 +87,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -91,7 +112,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -99,12 +120,214 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,577 +632,687 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11"/>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="18">
         <v>1.02</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="18">
+        <v>0</v>
+      </c>
+      <c r="D3" s="18">
         <v>0.78511545484343759</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="18">
         <v>0.148701100220169</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="F3" s="18">
+        <v>0</v>
+      </c>
+      <c r="G3" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="19">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="19">
         <v>1.0329999999999999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="19">
         <v>0.39890332031625919</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="19">
         <v>0.30000000000001981</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="19">
         <v>0.25640438071051008</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="F4" s="19">
+        <v>0</v>
+      </c>
+      <c r="G4" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="19">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="19">
         <v>1.0289999999999999</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="19">
         <v>-0.2850661730171532</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="19">
         <v>0.3300000000000114</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="19">
         <v>0.13755916629168399</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="F5" s="19">
+        <v>0</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="19">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="19">
         <v>0.98499999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="19">
         <v>-6.2039903187463308</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="19">
         <v>0.17999999999935709</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="19">
         <v>0.16573372887210169</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="F6" s="19">
+        <v>0</v>
+      </c>
+      <c r="G6" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="19">
         <v>0.96942421438987403</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="19">
         <v>-7.8605069271660533</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="19">
+        <v>0</v>
+      </c>
+      <c r="E7" s="19">
+        <v>0</v>
+      </c>
+      <c r="F7" s="19">
         <v>0.1000000000534715</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="19">
         <v>5.9999999985443253E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="19">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="19">
         <v>0.91238149724637241</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="19">
         <v>-16.633333216805731</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="19">
+        <v>0</v>
+      </c>
+      <c r="E8" s="19">
+        <v>0</v>
+      </c>
+      <c r="F8" s="19">
         <v>1.0499999999135361</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="19">
         <v>0.22499999992150421</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="19">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="19">
         <v>0.91358701669357245</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="19">
         <v>-16.297937125025928</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="19">
+        <v>0</v>
+      </c>
+      <c r="E9" s="19">
+        <v>0</v>
+      </c>
+      <c r="F9" s="19">
         <v>0.17999999993345739</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="19">
         <v>4.499999999308546E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="19">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="19">
         <v>0.92949600405712929</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="19">
         <v>-13.078364440086609</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="19">
+        <v>0</v>
+      </c>
+      <c r="E10" s="19">
+        <v>0</v>
+      </c>
+      <c r="F10" s="19">
         <v>0.22500000004330761</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="19">
         <v>4.4999999968148963E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="19">
         <v>1.5951154548428259</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="19">
         <v>0.70839837609446477</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="19">
         <v>1.5549999999437729</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="19">
         <v>0.37499999986818189</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="6"/>
+      <c r="E1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>-7.7627626278926012E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>-0.11667003600976911</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>7.7813130734147376E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>0.11272836546081071</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>1.8550445522136361E-4</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>1.9941728936296592E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>-7.7627626278926012E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>-0.11667003600976911</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>7.7813130734147376E-2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>0.11272836546081071</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>1.8550445522136361E-4</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>1.9941728936296592E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>0.14437373853170571</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>3.094764978896113E-2</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>-0.14420178393482869</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>-3.4014872716209961E-2</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>1.7195459687691089E-4</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="1">
         <v>1.8485119164265221E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>0.47420178393482848</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0.17157403900941659</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>-0.46905580677339292</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>-0.1281838304167896</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>5.1459771614355554E-3</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="1">
         <v>5.5319254485431929E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0.64905580677339358</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>0.29391755940363018</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>-0.64694080601927373</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>-0.27434454910289618</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>2.1150007541198561E-3</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="1">
         <v>2.3265008295317191E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>0.54694080601927353</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>0.21434454910289241</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>-0.54105110640216614</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>-0.1404453618443926</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>5.8896996171073912E-3</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="1">
         <v>9.4235193873717954E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>-2.547753155427657E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>-1.131856601308108E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>2.5487192725088769E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>-3.14266563913478E-3</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>9.661170812191866E-6</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="1">
         <v>1.545787329950759E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>-0.20548719272508881</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>-4.1857334360864383E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>0.20663353408133009</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>4.3860003767452839E-2</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>1.1463413562413931E-3</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="1">
         <v>1.232316957959499E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>1</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>0.4421014352426047</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>0.17660904548049311</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>-0.43163353408133021</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>-8.8860003767453011E-2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>1.0467901161274501E-2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="1">
         <v>0.1125299374837009</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>1</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>6</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>0.49826927222222023</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>0.20543212687405349</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>-0.48347136204355717</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>-7.3236072142526365E-2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>1.479791017866294E-2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="1">
         <v>0.159077534420627</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F14" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>4.0115454906973463E-2</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="1">
         <v>0.46274153457507078</v>
       </c>
     </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="20">
+        <f>C3+C4</f>
+        <v>-0.15525525255785202</v>
+      </c>
+      <c r="D17" s="20">
+        <f>D3+D4</f>
+        <v>-0.23334007201953821</v>
+      </c>
+      <c r="E17" s="20">
+        <f>E3+E4</f>
+        <v>0.15562626146829475</v>
+      </c>
+      <c r="F17" s="20">
+        <f>F3+F4</f>
+        <v>0.22545673092162141</v>
+      </c>
+      <c r="G17" s="20">
+        <f>G3+G4</f>
+        <v>3.7100891044272721E-4</v>
+      </c>
+      <c r="H17" s="20">
+        <f>H3+H4</f>
+        <v>3.9883457872593184E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f>C17*1000</f>
+        <v>-155.25525255785203</v>
+      </c>
+      <c r="D18">
+        <f>D17*1000</f>
+        <v>-233.34007201953821</v>
+      </c>
+      <c r="E18">
+        <f>E17*1000</f>
+        <v>155.62626146829476</v>
+      </c>
+      <c r="F18">
+        <f>F17*1000</f>
+        <v>225.45673092162141</v>
+      </c>
+      <c r="G18">
+        <f>G17*1000</f>
+        <v>0.37100891044272721</v>
+      </c>
+      <c r="H18">
+        <f>H17*1000</f>
+        <v>3.9883457872593184</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -990,9 +1323,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2.0337012033594739</v>
       </c>
@@ -1018,7 +1351,7 @@
         <v>-0.18244753366410449</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-1.685847079621144</v>
       </c>
@@ -1044,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1070,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1096,7 +1429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1122,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-0.1654065900742264</v>
       </c>
@@ -1148,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1174,7 +1507,7 @@
         <v>-0.39074795671380941</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-0.18244753366410449</v>
       </c>
@@ -1211,9 +1544,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-21.829288819668751</v>
       </c>
@@ -1239,7 +1572,7 @@
         <v>1.961310986889121</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>18.122856105927411</v>
       </c>
@@ -1265,7 +1598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1291,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1317,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1343,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.7781208432979341</v>
       </c>
@@ -1369,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1395,7 +1728,7 @@
         <v>4.2005405346734577</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.961310986889121</v>
       </c>

</xml_diff>

<commit_message>
Endra System_data til 4c)
</commit_message>
<xml_diff>
--- a/prosjektfiler/LoadFlow_results.xlsx
+++ b/prosjektfiler/LoadFlow_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arntzen/Desktop/IELET2118---Prosjekt-Lastflytanalyse/prosjektfiler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Desktop\IELET2118---Prosjekt-Lastflytanalyse\prosjektfiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DD0FAC-323E-EE41-94FA-4E526E1120EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC58FAF-745E-43A0-8450-2D14BA3A7855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus_information" sheetId="1" r:id="rId1"/>
@@ -74,8 +74,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -91,7 +99,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -99,12 +107,211 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,247 +617,274 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>1.02</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
         <v>0.78998657729434907</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="5">
         <v>1.11232309770952</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>0.98134999999999994</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.68685228352177674</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.30000000000001981</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>-1.2464689864270291</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>1.0289999999999999</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>-0.31157203760352181</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.33000000000001323</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0.73007287056553238</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>0.98499999999999999</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>-6.2241792650881171</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.17999999999935529</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>0.16561880216124791</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>0.96942645311559394</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>-7.87942420916574</v>
       </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2">
         <v>0.1000000000535408</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>5.9999999985443253E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>0.91237023859838695</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>-16.64444408055483</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2">
         <v>1.0499999999132059</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>0.22499999992128039</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>0.91356882197316391</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>-16.306714575270789</v>
       </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
         <v>0.17999999993315821</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>4.4999999993030393E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>0.92947400499751731</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>-13.08419507808039</v>
       </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
+      <c r="D10" s="2">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
         <v>0.22500000004357179</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>4.4999999967954452E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>1.5999865772937369</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>0.76154578400927164</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>1.5549999999434769</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>0.37499999986770849</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -659,325 +893,358 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="H1" s="4"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>-7.5439217228010252E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>0.3650645282051902</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>7.6819647265077617E-2</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>-0.35586771180286098</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>1.380430037067365E-3</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>1.4839622898474181E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>-7.5439217228010252E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.3650645282051902</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>7.6819647265077617E-2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>-0.35586771180286098</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>1.380430037067365E-3</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>1.4839622898474181E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.14636070546984431</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>-0.53473356282123286</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>-0.14371460835208991</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>0.55850394380971147</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>2.646097117754459E-3</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>2.8445544015859969E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.47371460835208973</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.17156892675742891</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>-0.46857793319244051</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>-0.12827871468400481</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>5.1366751596491622E-3</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>5.5219257966229091E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.64857793319244017</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0.29389751696035948</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>-0.64646555957183127</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>-0.27435341351842912</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>2.1123736206088979E-3</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>2.323610982669699E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0.54646555957183107</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0.21435341351842849</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>-0.54058456817480538</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>-0.14059337184631579</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>5.8809913970256922E-3</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>9.4095862352411824E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>-2.564942904547703E-2</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>-1.127382624638878E-2</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>2.5659212913510539E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>-3.1849706672091348E-3</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>9.7838680335089745E-6</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>1.5654188853618441E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>-0.20565921291351069</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>-4.1815029332791853E-2</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>0.20680737902568949</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>4.383776533193267E-2</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>1.1481661121788831E-3</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>1.234278570592252E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>8</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>0.44228376235544642</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.1766785225180933</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>-0.43180737902568939</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>-8.8837765331932134E-2</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>1.0476383329756979E-2</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>0.11262112079488711</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>1</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>6</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>0.49858124945879112</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>0.20551551889633851</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>-0.4837660027797176</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>-7.3132801907296818E-2</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>1.481524667907352E-2</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>0.15926390180004041</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F14" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>4.4986577358215832E-2</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>0.51506037014753236</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -988,9 +1255,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2.0337012033594739</v>
       </c>
@@ -1016,7 +1283,7 @@
         <v>-0.18244753366410449</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-1.685847079621144</v>
       </c>
@@ -1042,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1068,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1094,7 +1361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1120,7 +1387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-0.1654065900742264</v>
       </c>
@@ -1146,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1172,7 +1439,7 @@
         <v>-0.39074795671380941</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-0.18244753366410449</v>
       </c>
@@ -1209,9 +1476,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-21.829288819668751</v>
       </c>
@@ -1237,7 +1504,7 @@
         <v>1.961310986889121</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>18.122856105927411</v>
       </c>
@@ -1263,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1289,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1315,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1341,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.7781208432979341</v>
       </c>
@@ -1367,7 +1634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -1393,7 +1660,7 @@
         <v>4.2005405346734577</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.961310986889121</v>
       </c>

</xml_diff>